<commit_message>
use index culture date
</commit_message>
<xml_diff>
--- a/mssa_dem.xlsx
+++ b/mssa_dem.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/orca/Local/echidna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A646D30-C1DB-B542-BC52-41C5CEC2AA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79DAB5E-48D1-F240-AD97-1A0F410DCEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1260" windowWidth="27640" windowHeight="16740" xr2:uid="{C47497CF-E421-F44A-B625-D6D2A3F58CFC}"/>
+    <workbookView xWindow="0" yWindow="1260" windowWidth="27640" windowHeight="16740" xr2:uid="{C47497CF-E421-F44A-B625-D6D2A3F58CFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="1" r:id="rId1"/>
@@ -95,6 +95,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -124,8 +127,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,13 +447,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511EF759-B0E5-F84A-B729-E0995236FA91}">
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -511,10 +517,16 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="N2" s="1">
+        <v>44581.62222222222</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>2</v>
+      </c>
+      <c r="N3" s="2">
+        <v>44581</v>
       </c>
     </row>
   </sheetData>

</xml_diff>